<commit_message>
fix: createDataSet 경로 수정
</commit_message>
<xml_diff>
--- a/frontend/src/data/data0입학2021이수1학기.xlsx
+++ b/frontend/src/data/data0입학2021이수1학기.xlsx
@@ -555,7 +555,7 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>EGC2065</t>
+          <t>EGC3035</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -563,12 +563,12 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>글로벌한국사</t>
+          <t>바이오의료산업경영</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>김성연</t>
+          <t>권지연</t>
         </is>
       </c>
       <c r="J2" t="n">
@@ -576,7 +576,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>B+</t>
+          <t>B0</t>
         </is>
       </c>
       <c r="L2" t="inlineStr"/>
@@ -589,7 +589,7 @@
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr">
         <is>
-          <t>Global Korean History</t>
+          <t>Introduction to Health Industry Management</t>
         </is>
       </c>
       <c r="U2" t="inlineStr"/>
@@ -614,7 +614,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>EGC2104</t>
+          <t>EGC4023</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -622,12 +622,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>IntroductiontotheHistoryofModernArt</t>
+          <t>인간과우주</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>캐서린무어</t>
+          <t>이관수</t>
         </is>
       </c>
       <c r="J3" t="n">
@@ -635,7 +635,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>C+</t>
+          <t>A0</t>
         </is>
       </c>
       <c r="L3" t="inlineStr"/>
@@ -647,16 +647,12 @@
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>영어</t>
-        </is>
-      </c>
+      <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr">
         <is>
-          <t>Introduction to the History of Modern Art</t>
+          <t>Humanity and Universe</t>
         </is>
       </c>
       <c r="U3" t="inlineStr"/>

</xml_diff>